<commit_message>
added some header that made sense
</commit_message>
<xml_diff>
--- a/naiveBayes.xlsx
+++ b/naiveBayes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
   <si>
     <t>Row #</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Class Conditionals</t>
+  </si>
+  <si>
+    <t>Yes(Prob)</t>
+  </si>
+  <si>
+    <t>No (Prob)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="B2:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +497,7 @@
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,10 +527,10 @@
         <v>13</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">

</xml_diff>